<commit_message>
contains only corrected data -- old data have been archived to incorrect/ folder
</commit_message>
<xml_diff>
--- a/Final-Corpus-Transcripts-Annotations-Data/Group-Individual-Data/Group-Level Meeting Data.xlsx
+++ b/Final-Corpus-Transcripts-Annotations-Data/Group-Individual-Data/Group-Level Meeting Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Meeting</t>
   </si>
@@ -37,31 +37,19 @@
     <t xml:space="preserve">Group_TE</t>
   </si>
   <si>
-    <t xml:space="preserve">Group_TE_Changed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Group_WW</t>
   </si>
   <si>
     <t xml:space="preserve">Group_TM</t>
   </si>
   <si>
-    <t xml:space="preserve">Group_TM_Changed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Group_Eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group_Eff_Changed</t>
   </si>
   <si>
     <t xml:space="preserve">Group_QW</t>
   </si>
   <si>
     <t xml:space="preserve">Group_Sat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group_Sat_Changed</t>
   </si>
 </sst>
 </file>
@@ -206,21 +194,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="15" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="30" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="11" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="26" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -254,18 +248,6 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
@@ -284,30 +266,18 @@
         <v>4.67</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>4.67</v>
+        <v>5</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>5</v>
       </c>
       <c r="H2" s="4" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J2" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>4.87</v>
-      </c>
-      <c r="N2" s="5" t="n">
+      <c r="J2" s="5" t="n">
         <v>4.87</v>
       </c>
     </row>
@@ -331,27 +301,15 @@
         <v>4.5</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J3" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L3" s="5" t="n">
+      <c r="I3" s="5" t="n">
         <v>4.5</v>
       </c>
-      <c r="M3" s="5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="N3" s="5" t="n">
+      <c r="J3" s="5" t="n">
         <v>4.7</v>
       </c>
     </row>
@@ -378,24 +336,12 @@
         <v>4.5</v>
       </c>
       <c r="H4" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5" t="n">
         <v>4.5</v>
       </c>
-      <c r="I4" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K4" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="N4" s="5" t="n">
+      <c r="J4" s="5" t="n">
         <v>4.6</v>
       </c>
     </row>
@@ -416,30 +362,18 @@
         <v>4.67</v>
       </c>
       <c r="F5" s="4" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="G5" s="4" t="n">
         <v>4.67</v>
       </c>
-      <c r="G5" s="4" t="n">
-        <v>4.33</v>
-      </c>
       <c r="H5" s="4" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="I5" s="5" t="n">
         <v>4.67</v>
       </c>
-      <c r="I5" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="J5" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>4.53</v>
-      </c>
-      <c r="N5" s="5" t="n">
+      <c r="J5" s="5" t="n">
         <v>4.53</v>
       </c>
     </row>
@@ -460,30 +394,18 @@
         <v>3.25</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="H6" s="4" t="n">
         <v>4.25</v>
       </c>
-      <c r="I6" s="4" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="J6" s="4" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="K6" s="4" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="L6" s="5" t="n">
+      <c r="I6" s="5" t="n">
         <v>3.75</v>
       </c>
-      <c r="M6" s="5" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="N6" s="5" t="n">
+      <c r="J6" s="5" t="n">
         <v>3.9</v>
       </c>
     </row>
@@ -507,27 +429,15 @@
         <v>4.75</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="H7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J7" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L7" s="5" t="n">
+      <c r="I7" s="5" t="n">
         <v>4.75</v>
       </c>
-      <c r="M7" s="5" t="n">
-        <v>4.85</v>
-      </c>
-      <c r="N7" s="5" t="n">
+      <c r="J7" s="5" t="n">
         <v>4.85</v>
       </c>
     </row>
@@ -548,30 +458,18 @@
         <v>3</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>3</v>
+        <v>4.67</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>4.67</v>
+        <v>4.33</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="I8" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="J8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K8" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="N8" s="5" t="n">
+      <c r="I8" s="5" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J8" s="5" t="n">
         <v>4.27</v>
       </c>
     </row>
@@ -592,30 +490,18 @@
         <v>4</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>4</v>
+        <v>4.67</v>
       </c>
       <c r="G9" s="4" t="n">
         <v>4.67</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="I9" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="J9" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K9" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>4.53</v>
-      </c>
-      <c r="N9" s="5" t="n">
+      <c r="I9" s="5" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J9" s="5" t="n">
         <v>4.53</v>
       </c>
     </row>
@@ -644,22 +530,10 @@
       <c r="H10" s="4" t="n">
         <v>4.33</v>
       </c>
-      <c r="I10" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="J10" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="K10" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="L10" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M10" s="5" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="N10" s="5" t="n">
+      <c r="I10" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" s="5" t="n">
         <v>4.27</v>
       </c>
     </row>
@@ -680,30 +554,18 @@
         <v>5</v>
       </c>
       <c r="F11" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G11" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H11" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I11" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="J11" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K11" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L11" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M11" s="5" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="N11" s="5" t="n">
+      <c r="I11" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" s="5" t="n">
         <v>4.5</v>
       </c>
     </row>
@@ -724,30 +586,18 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I12" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="J12" s="4" t="n">
         <v>1.5</v>
       </c>
-      <c r="K12" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="L12" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M12" s="5" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="N12" s="5" t="n">
+      <c r="I12" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" s="5" t="n">
         <v>3.3</v>
       </c>
     </row>
@@ -768,30 +618,18 @@
         <v>4.25</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>4.25</v>
+        <v>4.75</v>
       </c>
       <c r="G13" s="4" t="n">
         <v>4.75</v>
       </c>
       <c r="H13" s="4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I13" s="5" t="n">
         <v>4.75</v>
       </c>
-      <c r="I13" s="4" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="J13" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="K13" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L13" s="5" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="M13" s="5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="N13" s="5" t="n">
+      <c r="J13" s="5" t="n">
         <v>4.6</v>
       </c>
     </row>
@@ -812,30 +650,18 @@
         <v>4</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="H14" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I14" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J14" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="K14" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="L14" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M14" s="5" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="N14" s="5" t="n">
+      <c r="I14" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J14" s="5" t="n">
         <v>4.1</v>
       </c>
     </row>
@@ -853,33 +679,21 @@
         <v>62</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>1.5</v>
+        <v>4.25</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>4.25</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>4.25</v>
+        <v>4.75</v>
       </c>
       <c r="H15" s="4" t="n">
         <v>4.75</v>
       </c>
-      <c r="I15" s="4" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="J15" s="4" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="K15" s="4" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="L15" s="6" t="n">
+      <c r="I15" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="M15" s="6" t="n">
-        <v>3.95</v>
-      </c>
-      <c r="N15" s="6" t="n">
+      <c r="J15" s="6" t="n">
         <v>4.5</v>
       </c>
     </row>
@@ -897,33 +711,21 @@
         <v>78</v>
       </c>
       <c r="E16" s="4" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4" t="n">
         <v>3.75</v>
       </c>
-      <c r="F16" s="4" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="G16" s="4" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="H16" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="I16" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J16" s="4" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="K16" s="4" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="L16" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="M16" s="6" t="n">
-        <v>4.05</v>
-      </c>
-      <c r="N16" s="6" t="n">
+      <c r="I16" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="J16" s="6" t="n">
         <v>3.75</v>
       </c>
     </row>
@@ -941,33 +743,21 @@
         <v>64</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>1.67</v>
+        <v>4.33</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>4.67</v>
+        <v>4.33</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="I17" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="J17" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K17" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L17" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M17" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N17" s="6" t="n">
+      <c r="I17" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J17" s="6" t="n">
         <v>4.53</v>
       </c>
     </row>
@@ -985,33 +775,21 @@
         <v>76</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="I18" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J18" s="4" t="n">
         <v>4.25</v>
       </c>
-      <c r="K18" s="4" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="L18" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="M18" s="6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="N18" s="6" t="n">
+      <c r="I18" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="J18" s="6" t="n">
         <v>4.15</v>
       </c>
     </row>
@@ -1029,33 +807,21 @@
         <v>84</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>3.67</v>
+        <v>2.33</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>2.33</v>
+        <v>2.83</v>
       </c>
       <c r="G19" s="4" t="n">
         <v>2.83</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="I19" s="4" t="n">
         <v>2.83</v>
       </c>
-      <c r="J19" s="4" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="K19" s="4" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="L19" s="6" t="n">
+      <c r="I19" s="6" t="n">
         <v>2.5</v>
       </c>
-      <c r="M19" s="6" t="n">
-        <v>2.93</v>
-      </c>
-      <c r="N19" s="6" t="n">
+      <c r="J19" s="6" t="n">
         <v>2.67</v>
       </c>
     </row>
@@ -1073,33 +839,21 @@
         <v>88</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>1.67</v>
+        <v>4.33</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="G20" s="4" t="n">
         <v>4.67</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="I20" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="J20" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K20" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L20" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M20" s="6" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="N20" s="6" t="n">
+      <c r="I20" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J20" s="6" t="n">
         <v>4.6</v>
       </c>
     </row>
@@ -1117,33 +871,21 @@
         <v>76</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>2.67</v>
+        <v>3.33</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>3.33</v>
+        <v>4.33</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>4.33</v>
+        <v>5</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I21" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J21" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K21" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L21" s="6" t="n">
+      <c r="I21" s="6" t="n">
         <v>4.67</v>
       </c>
-      <c r="M21" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="N21" s="6" t="n">
+      <c r="J21" s="6" t="n">
         <v>4.47</v>
       </c>
     </row>
@@ -1161,33 +903,21 @@
         <v>80</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>1.67</v>
+        <v>4.33</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>4.33</v>
+        <v>5</v>
       </c>
       <c r="G22" s="4" t="n">
         <v>5</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="I22" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J22" s="4" t="n">
         <v>3.33</v>
       </c>
-      <c r="K22" s="4" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="L22" s="6" t="n">
+      <c r="I22" s="6" t="n">
         <v>4.67</v>
       </c>
-      <c r="M22" s="6" t="n">
-        <v>3.93</v>
-      </c>
-      <c r="N22" s="6" t="n">
+      <c r="J22" s="6" t="n">
         <v>4.47</v>
       </c>
     </row>
@@ -1205,10 +935,10 @@
         <v>66</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>2.33</v>
+        <v>3.67</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>3.67</v>
+        <v>4.67</v>
       </c>
       <c r="G23" s="4" t="n">
         <v>4.67</v>
@@ -1216,22 +946,10 @@
       <c r="H23" s="4" t="n">
         <v>4.67</v>
       </c>
-      <c r="I23" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="J23" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="K23" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="L23" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M23" s="6" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="N23" s="6" t="n">
+      <c r="I23" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J23" s="6" t="n">
         <v>4.4</v>
       </c>
     </row>
@@ -1249,33 +967,21 @@
         <v>90</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="F24" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4" t="n">
         <v>4.5</v>
-      </c>
-      <c r="G24" s="4" t="n">
-        <v>5</v>
       </c>
       <c r="H24" s="4" t="n">
         <v>4.5</v>
       </c>
-      <c r="I24" s="4" t="n">
+      <c r="I24" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="J24" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="K24" s="4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L24" s="6" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="M24" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N24" s="6" t="n">
+      <c r="J24" s="6" t="n">
         <v>4.6</v>
       </c>
     </row>
@@ -1293,33 +999,21 @@
         <v>47</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>2.33</v>
+        <v>3.67</v>
       </c>
       <c r="F25" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" s="4" t="n">
         <v>3.67</v>
       </c>
-      <c r="G25" s="4" t="n">
-        <v>4</v>
-      </c>
       <c r="H25" s="4" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="I25" s="4" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="J25" s="4" t="n">
         <v>4.67</v>
       </c>
-      <c r="K25" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="L25" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M25" s="6" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="N25" s="6" t="n">
+      <c r="I25" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J25" s="6" t="n">
         <v>4.07</v>
       </c>
     </row>
@@ -1337,7 +1031,7 @@
         <v>100</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>4</v>
@@ -1346,24 +1040,12 @@
         <v>4</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="I26" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J26" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="K26" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="L26" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M26" s="6" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="N26" s="6" t="n">
+      <c r="I26" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J26" s="6" t="n">
         <v>3.87</v>
       </c>
     </row>
@@ -1381,33 +1063,21 @@
         <v>92</v>
       </c>
       <c r="E27" s="4" t="n">
-        <v>2.33</v>
+        <v>3.33</v>
       </c>
       <c r="F27" s="4" t="n">
-        <v>3.33</v>
+        <v>3.67</v>
       </c>
       <c r="G27" s="4" t="n">
-        <v>3.67</v>
+        <v>4.33</v>
       </c>
       <c r="H27" s="4" t="n">
         <v>4.33</v>
       </c>
-      <c r="I27" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="J27" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="K27" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="L27" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M27" s="6" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="N27" s="6" t="n">
+      <c r="I27" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J27" s="6" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1425,33 +1095,21 @@
         <v>66</v>
       </c>
       <c r="E28" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F28" s="4" t="n">
-        <v>4</v>
+        <v>4.67</v>
       </c>
       <c r="G28" s="4" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H28" s="4" t="n">
         <v>4.67</v>
       </c>
-      <c r="H28" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="I28" s="4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="J28" s="4" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="K28" s="4" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="L28" s="6" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="M28" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N28" s="6" t="n">
+      <c r="I28" s="6" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J28" s="6" t="n">
         <v>4.4</v>
       </c>
     </row>
@@ -1469,33 +1127,21 @@
         <v>72</v>
       </c>
       <c r="E29" s="8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F29" s="8" t="n">
         <v>4</v>
       </c>
       <c r="G29" s="8" t="n">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="H29" s="8" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="I29" s="8" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="J29" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="K29" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="L29" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I29" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="M29" s="6" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="N29" s="6" t="n">
+      <c r="J29" s="6" t="n">
         <v>4.2</v>
       </c>
     </row>

</xml_diff>